<commit_message>
Seed for part number
</commit_message>
<xml_diff>
--- a/documents/templates/bulk-upload/14-BulkUploadPartNumberTemplate-s2.xlsx
+++ b/documents/templates/bulk-upload/14-BulkUploadPartNumberTemplate-s2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EA0D57-EFC0-4749-B42E-1DDEE370B6E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EF5C4E-0EE8-4730-94E5-CAE4ED52CB6F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27080" windowHeight="14000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="28">
   <si>
     <t>PartNumber</t>
   </si>
@@ -89,6 +89,21 @@
   </si>
   <si>
     <t>Raw Material Number</t>
+  </si>
+  <si>
+    <t>process _6</t>
+  </si>
+  <si>
+    <t>process _7</t>
+  </si>
+  <si>
+    <t>process _8</t>
+  </si>
+  <si>
+    <t>process _9</t>
+  </si>
+  <si>
+    <t>process _10</t>
   </si>
 </sst>
 </file>
@@ -451,39 +466,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD26"/>
+  <dimension ref="A1:BC26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:55" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -574,8 +589,83 @@
       <c r="AD1" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AP1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AT1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AX1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AY1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AZ1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="BA1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="BC1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>922101700022</v>
       </c>
@@ -639,7 +729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>922100200162</v>
       </c>
@@ -695,7 +785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>923100400259</v>
       </c>
@@ -751,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>921105700028</v>
       </c>
@@ -807,7 +897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>922100300118</v>
       </c>
@@ -871,7 +961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>399028083665</v>
       </c>
@@ -935,7 +1025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>319028083349</v>
       </c>
@@ -999,7 +1089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>319028083352</v>
       </c>
@@ -1063,7 +1153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>319028083351</v>
       </c>
@@ -1127,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>921100800310</v>
       </c>
@@ -1183,7 +1273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>379003004284</v>
       </c>
@@ -1235,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>921100800019</v>
       </c>
@@ -1291,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>921100800020</v>
       </c>
@@ -1347,7 +1437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>921100900039</v>
       </c>
@@ -1403,7 +1493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>921102300101</v>
       </c>
@@ -1459,7 +1549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>379003004035</v>
       </c>
@@ -1511,7 +1601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>921103300113</v>
       </c>
@@ -1567,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>921103300342</v>
       </c>
@@ -1623,7 +1713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>399016085002</v>
       </c>
@@ -1679,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>922101800034</v>
       </c>
@@ -1743,7 +1833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>921100800386</v>
       </c>
@@ -1799,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>399028083634</v>
       </c>
@@ -1863,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>921100800423</v>
       </c>
@@ -1919,7 +2009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>399003013730</v>
       </c>
@@ -1975,7 +2065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>319028083304</v>
       </c>

</xml_diff>